<commit_message>
Updated Corrected Weather Data
</commit_message>
<xml_diff>
--- a/data/weather.xlsx
+++ b/data/weather.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12077\Documents\Masters\CS5500\Group-Project\CS5500\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EA1540-3937-4D48-8303-7260F966BFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1585FF-C5EE-4E54-8812-7E654A85F922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{24323D40-DFB7-4A42-9556-FAAE0CDFD06E}"/>
   </bookViews>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32200945-1671-4A27-87AC-AD2DF60C2160}">
   <dimension ref="A6:F294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
+      <selection activeCell="B296" sqref="B296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>40544</v>
+        <v>40909</v>
       </c>
       <c r="B151">
         <v>26.9</v>
@@ -3348,7 +3348,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>40575</v>
+        <v>40940</v>
       </c>
       <c r="B152">
         <v>30.5</v>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>40603</v>
+        <v>40969</v>
       </c>
       <c r="B153">
         <v>41.1</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>40634</v>
+        <v>41000</v>
       </c>
       <c r="B154">
         <v>47</v>
@@ -3408,7 +3408,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>40664</v>
+        <v>41030</v>
       </c>
       <c r="B155">
         <v>56.6</v>
@@ -3428,7 +3428,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>40695</v>
+        <v>41061</v>
       </c>
       <c r="B156">
         <v>63.2</v>
@@ -3448,7 +3448,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>40725</v>
+        <v>41091</v>
       </c>
       <c r="B157">
         <v>71.3</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>40909</v>
+        <v>41275</v>
       </c>
       <c r="B163">
         <v>25.4</v>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>40940</v>
+        <v>41306</v>
       </c>
       <c r="B164">
         <v>28</v>
@@ -3608,7 +3608,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>40969</v>
+        <v>41334</v>
       </c>
       <c r="B165">
         <v>34.799999999999997</v>
@@ -3628,7 +3628,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>41000</v>
+        <v>41365</v>
       </c>
       <c r="B166">
         <v>44.2</v>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>41030</v>
+        <v>41395</v>
       </c>
       <c r="B167">
         <v>54.1</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>41061</v>
+        <v>41426</v>
       </c>
       <c r="B168">
         <v>64.8</v>
@@ -3808,7 +3808,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>41275</v>
+        <v>41640</v>
       </c>
       <c r="B175">
         <v>21.4</v>
@@ -3828,7 +3828,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>41306</v>
+        <v>41671</v>
       </c>
       <c r="B176">
         <v>22.1</v>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>41334</v>
+        <v>41699</v>
       </c>
       <c r="B177">
         <v>27</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>41365</v>
+        <v>41730</v>
       </c>
       <c r="B178">
         <v>43.3</v>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>41395</v>
+        <v>41760</v>
       </c>
       <c r="B179">
         <v>54.7</v>
@@ -3908,7 +3908,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>41426</v>
+        <v>41791</v>
       </c>
       <c r="B180">
         <v>64.099999999999994</v>
@@ -4048,7 +4048,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>41640</v>
+        <v>42005</v>
       </c>
       <c r="B187">
         <v>21.1</v>
@@ -4068,7 +4068,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>41671</v>
+        <v>42036</v>
       </c>
       <c r="B188">
         <v>13.8</v>
@@ -4088,7 +4088,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>41699</v>
+        <v>42064</v>
       </c>
       <c r="B189">
         <v>30.2</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>41730</v>
+        <v>42095</v>
       </c>
       <c r="B190">
         <v>44.7</v>
@@ -4128,7 +4128,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>41760</v>
+        <v>42125</v>
       </c>
       <c r="B191">
         <v>59.5</v>
@@ -4148,7 +4148,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>41791</v>
+        <v>42156</v>
       </c>
       <c r="B192">
         <v>61.4</v>
@@ -4288,7 +4288,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>42005</v>
+        <v>42370</v>
       </c>
       <c r="B199">
         <v>27</v>
@@ -4308,7 +4308,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>42036</v>
+        <v>42401</v>
       </c>
       <c r="B200">
         <v>28.8</v>
@@ -4328,7 +4328,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>42064</v>
+        <v>42430</v>
       </c>
       <c r="B201">
         <v>37.799999999999997</v>
@@ -4348,7 +4348,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>42095</v>
+        <v>42461</v>
       </c>
       <c r="B202">
         <v>42.7</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>42125</v>
+        <v>42491</v>
       </c>
       <c r="B203">
         <v>54.7</v>
@@ -4388,7 +4388,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>42156</v>
+        <v>42522</v>
       </c>
       <c r="B204">
         <v>63.7</v>
@@ -4528,7 +4528,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>42370</v>
+        <v>42736</v>
       </c>
       <c r="B211">
         <v>29.8</v>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>42401</v>
+        <v>42767</v>
       </c>
       <c r="B212">
         <v>28.7</v>
@@ -4568,7 +4568,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>42430</v>
+        <v>42795</v>
       </c>
       <c r="B213">
         <v>28.8</v>
@@ -4588,7 +4588,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>42461</v>
+        <v>42826</v>
       </c>
       <c r="B214">
         <v>46.7</v>
@@ -4608,7 +4608,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>42491</v>
+        <v>42856</v>
       </c>
       <c r="B215">
         <v>52.9</v>
@@ -4628,7 +4628,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>42522</v>
+        <v>42887</v>
       </c>
       <c r="B216">
         <v>65</v>
@@ -4768,7 +4768,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>42736</v>
+        <v>43101</v>
       </c>
       <c r="B223">
         <v>21.9</v>
@@ -4788,7 +4788,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>42767</v>
+        <v>43132</v>
       </c>
       <c r="B224">
         <v>31.6</v>
@@ -4808,7 +4808,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>42795</v>
+        <v>43160</v>
       </c>
       <c r="B225">
         <v>34</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>42826</v>
+        <v>43191</v>
       </c>
       <c r="B226">
         <v>41.8</v>
@@ -4848,7 +4848,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>42856</v>
+        <v>43221</v>
       </c>
       <c r="B227">
         <v>57.4</v>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>42887</v>
+        <v>43252</v>
       </c>
       <c r="B228">
         <v>63.5</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B235">
         <v>23.4</v>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>43132</v>
+        <v>43497</v>
       </c>
       <c r="B236">
         <v>26</v>
@@ -5048,7 +5048,7 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>43160</v>
+        <v>43525</v>
       </c>
       <c r="B237">
         <v>32</v>
@@ -5068,7 +5068,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>43191</v>
+        <v>43556</v>
       </c>
       <c r="B238">
         <v>44.7</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>43221</v>
+        <v>43586</v>
       </c>
       <c r="B239">
         <v>53</v>
@@ -5108,7 +5108,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>43252</v>
+        <v>43617</v>
       </c>
       <c r="B240">
         <v>62.8</v>
@@ -5248,7 +5248,7 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B247">
         <v>29.8</v>
@@ -5268,7 +5268,7 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>43497</v>
+        <v>43862</v>
       </c>
       <c r="B248">
         <v>29.8</v>
@@ -5288,7 +5288,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>43525</v>
+        <v>43891</v>
       </c>
       <c r="B249">
         <v>39</v>
@@ -5308,7 +5308,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>43556</v>
+        <v>43922</v>
       </c>
       <c r="B250">
         <v>42.5</v>
@@ -5328,7 +5328,7 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B251">
         <v>54.4</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
-        <v>43617</v>
+        <v>43983</v>
       </c>
       <c r="B252">
         <v>66.2</v>
@@ -5488,7 +5488,7 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>43831</v>
+        <v>44197</v>
       </c>
       <c r="B259">
         <v>27.8</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>43862</v>
+        <v>44228</v>
       </c>
       <c r="B260">
         <v>25.6</v>
@@ -5528,7 +5528,7 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>43891</v>
+        <v>44256</v>
       </c>
       <c r="B261">
         <v>34.9</v>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>43922</v>
+        <v>44287</v>
       </c>
       <c r="B262">
         <v>45.7</v>
@@ -5568,7 +5568,7 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
-        <v>43952</v>
+        <v>44317</v>
       </c>
       <c r="B263">
         <v>55.9</v>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>43983</v>
+        <v>44348</v>
       </c>
       <c r="B264">
         <v>68.900000000000006</v>
@@ -5728,7 +5728,7 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
-        <v>44197</v>
+        <v>44562</v>
       </c>
       <c r="B271">
         <v>20.6</v>
@@ -5748,7 +5748,7 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B272">
         <v>27.7</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
-        <v>44256</v>
+        <v>44621</v>
       </c>
       <c r="B273">
         <v>35.700000000000003</v>
@@ -5788,7 +5788,7 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
-        <v>44287</v>
+        <v>44652</v>
       </c>
       <c r="B274">
         <v>44.9</v>
@@ -5808,7 +5808,7 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
-        <v>44317</v>
+        <v>44682</v>
       </c>
       <c r="B275">
         <v>55.7</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
-        <v>44348</v>
+        <v>44713</v>
       </c>
       <c r="B276">
         <v>62.9</v>
@@ -5968,7 +5968,7 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
-        <v>44562</v>
+        <v>44927</v>
       </c>
       <c r="B283">
         <v>31.5</v>
@@ -5988,7 +5988,7 @@
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
-        <v>44593</v>
+        <v>44958</v>
       </c>
       <c r="B284">
         <v>27.1</v>
@@ -6008,7 +6008,7 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
-        <v>44621</v>
+        <v>44986</v>
       </c>
       <c r="B285">
         <v>35.700000000000003</v>
@@ -6028,7 +6028,7 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
-        <v>44652</v>
+        <v>45017</v>
       </c>
       <c r="B286">
         <v>45.2</v>
@@ -6048,7 +6048,7 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
-        <v>44682</v>
+        <v>45047</v>
       </c>
       <c r="B287">
         <v>55</v>
@@ -6068,7 +6068,7 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
-        <v>44713</v>
+        <v>45078</v>
       </c>
       <c r="B288">
         <v>61.3</v>

</xml_diff>